<commit_message>
Adding Json data testing related file...please note it also has excel reader and all, we can remove it later...
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/ExcelTestData.xlsx
+++ b/src/test/resources/TestData/ExcelTestData.xlsx
@@ -93,11 +93,12 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="xr9">
-  <numFmts count="4">
+  <numFmts count="5">
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="\20\2\4\-0\7\-\2\6\T\1\8\:\1\4\:0\8.\5\70\Z"/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -702,14 +703,17 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="6" applyAlignment="1">
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="6" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1255,7 +1259,7 @@
   <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.703125" defaultRowHeight="16.8" outlineLevelRow="1"/>
@@ -1264,7 +1268,7 @@
     <col min="2" max="16384" width="20.703125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="17" spans="1:11">
+    <row r="1" s="1" customFormat="1" ht="17" spans="1:11">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1299,20 +1303,20 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" ht="34" spans="1:11">
+    <row r="2" s="1" customFormat="1" ht="34" spans="1:11">
       <c r="A2" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B2" s="1">
         <v>3344557765</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="2" t="s">
         <v>12</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="3" t="s">
         <v>14</v>
       </c>
       <c r="F2" s="1" t="s">

</xml_diff>